<commit_message>
Added more trial xls files.
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/cue_dis_ch1.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/cue_dis_ch1.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="7">
   <si>
     <t xml:space="preserve">Left_Cue</t>
   </si>
   <si>
     <t xml:space="preserve">Right_Cue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training_mode</t>
   </si>
   <si>
     <t xml:space="preserve">Circle</t>
@@ -47,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -82,11 +85,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +129,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -145,10 +143,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,10 +166,10 @@
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -184,863 +178,866 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>